<commit_message>
Fixing change user group
</commit_message>
<xml_diff>
--- a/src/core/data/EBOM.xlsx
+++ b/src/core/data/EBOM.xlsx
@@ -513,7 +513,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -634,10 +634,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -697,14 +693,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
+          <fgColor rgb="00FFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <fgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1027,7 +1023,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="17:17"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1082,7 +1078,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="5" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="67" min="67" style="5" width="15.44"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="68" min="68" style="5" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="69" min="69" style="5" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="69" min="69" style="5" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="70" min="70" style="5" width="16.66"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="71" min="71" style="5" width="13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="72" min="72" style="5" width="64"/>
@@ -1096,7 +1092,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="8" width="10.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="8" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="8" width="13.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="85" min="85" style="8" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="85" min="85" style="8" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="86" min="86" style="5" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="87" min="87" style="8" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="88" min="88" style="8" width="6.55"/>
@@ -1382,7 +1378,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="24" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" s="24" t="n">
         <v>12</v>
@@ -1505,39 +1501,39 @@
         <v>103</v>
       </c>
       <c r="BV2" s="24"/>
-      <c r="BW2" s="30" t="s">
+      <c r="BW2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX2" s="31" t="s">
+      <c r="BX2" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY2" s="30" t="s">
+      <c r="BY2" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ2" s="30" t="s">
+      <c r="BZ2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA2" s="30" t="s">
+      <c r="CA2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB2" s="32"/>
+      <c r="CB2" s="31"/>
       <c r="CC2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD2" s="32"/>
-      <c r="CE2" s="32"/>
-      <c r="CF2" s="32" t="s">
+      <c r="CD2" s="31"/>
+      <c r="CE2" s="31"/>
+      <c r="CF2" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG2" s="32"/>
-      <c r="CH2" s="32" t="s">
+      <c r="CG2" s="31"/>
+      <c r="CH2" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI2" s="32"/>
-      <c r="CJ2" s="33"/>
-      <c r="CK2" s="33"/>
-      <c r="CL2" s="33"/>
-      <c r="CM2" s="34" t="n">
+      <c r="CI2" s="31"/>
+      <c r="CJ2" s="32"/>
+      <c r="CK2" s="32"/>
+      <c r="CL2" s="32"/>
+      <c r="CM2" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1669,39 +1665,39 @@
         <v>103</v>
       </c>
       <c r="BV3" s="24"/>
-      <c r="BW3" s="30" t="s">
+      <c r="BW3" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX3" s="31" t="s">
+      <c r="BX3" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY3" s="30" t="s">
+      <c r="BY3" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ3" s="30" t="s">
+      <c r="BZ3" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA3" s="30" t="s">
+      <c r="CA3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB3" s="32"/>
+      <c r="CB3" s="31"/>
       <c r="CC3" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD3" s="32"/>
-      <c r="CE3" s="32"/>
-      <c r="CF3" s="32" t="s">
+      <c r="CD3" s="31"/>
+      <c r="CE3" s="31"/>
+      <c r="CF3" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG3" s="32"/>
-      <c r="CH3" s="32" t="s">
+      <c r="CG3" s="31"/>
+      <c r="CH3" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI3" s="32"/>
-      <c r="CJ3" s="33"/>
-      <c r="CK3" s="33"/>
-      <c r="CL3" s="33"/>
-      <c r="CM3" s="34" t="n">
+      <c r="CI3" s="31"/>
+      <c r="CJ3" s="32"/>
+      <c r="CK3" s="32"/>
+      <c r="CL3" s="32"/>
+      <c r="CM3" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1833,39 +1829,39 @@
         <v>103</v>
       </c>
       <c r="BV4" s="24"/>
-      <c r="BW4" s="30" t="s">
+      <c r="BW4" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX4" s="31" t="s">
+      <c r="BX4" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY4" s="30" t="s">
+      <c r="BY4" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ4" s="30" t="s">
+      <c r="BZ4" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA4" s="30" t="s">
+      <c r="CA4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB4" s="32"/>
+      <c r="CB4" s="31"/>
       <c r="CC4" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD4" s="32"/>
-      <c r="CE4" s="32"/>
-      <c r="CF4" s="32" t="s">
+      <c r="CD4" s="31"/>
+      <c r="CE4" s="31"/>
+      <c r="CF4" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG4" s="32"/>
-      <c r="CH4" s="32" t="s">
+      <c r="CG4" s="31"/>
+      <c r="CH4" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI4" s="32"/>
-      <c r="CJ4" s="33"/>
-      <c r="CK4" s="33"/>
-      <c r="CL4" s="33"/>
-      <c r="CM4" s="34" t="n">
+      <c r="CI4" s="31"/>
+      <c r="CJ4" s="32"/>
+      <c r="CK4" s="32"/>
+      <c r="CL4" s="32"/>
+      <c r="CM4" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1997,39 +1993,39 @@
         <v>103</v>
       </c>
       <c r="BV5" s="24"/>
-      <c r="BW5" s="30" t="s">
+      <c r="BW5" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX5" s="31" t="s">
+      <c r="BX5" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY5" s="30" t="s">
+      <c r="BY5" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ5" s="30" t="s">
+      <c r="BZ5" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA5" s="30" t="s">
+      <c r="CA5" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB5" s="32"/>
+      <c r="CB5" s="31"/>
       <c r="CC5" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD5" s="32"/>
-      <c r="CE5" s="32"/>
-      <c r="CF5" s="32" t="s">
+      <c r="CD5" s="31"/>
+      <c r="CE5" s="31"/>
+      <c r="CF5" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG5" s="32"/>
-      <c r="CH5" s="32" t="s">
+      <c r="CG5" s="31"/>
+      <c r="CH5" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI5" s="32"/>
-      <c r="CJ5" s="33"/>
-      <c r="CK5" s="33"/>
-      <c r="CL5" s="33"/>
-      <c r="CM5" s="34" t="n">
+      <c r="CI5" s="31"/>
+      <c r="CJ5" s="32"/>
+      <c r="CK5" s="32"/>
+      <c r="CL5" s="32"/>
+      <c r="CM5" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2161,39 +2157,39 @@
         <v>103</v>
       </c>
       <c r="BV6" s="24"/>
-      <c r="BW6" s="30" t="s">
+      <c r="BW6" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX6" s="31" t="s">
+      <c r="BX6" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY6" s="30" t="s">
+      <c r="BY6" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ6" s="30" t="s">
+      <c r="BZ6" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA6" s="30" t="s">
+      <c r="CA6" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB6" s="32"/>
+      <c r="CB6" s="31"/>
       <c r="CC6" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD6" s="32"/>
-      <c r="CE6" s="32"/>
-      <c r="CF6" s="32" t="s">
+      <c r="CD6" s="31"/>
+      <c r="CE6" s="31"/>
+      <c r="CF6" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG6" s="32"/>
-      <c r="CH6" s="32" t="s">
+      <c r="CG6" s="31"/>
+      <c r="CH6" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI6" s="32"/>
-      <c r="CJ6" s="33"/>
-      <c r="CK6" s="33"/>
-      <c r="CL6" s="33"/>
-      <c r="CM6" s="34" t="n">
+      <c r="CI6" s="31"/>
+      <c r="CJ6" s="32"/>
+      <c r="CK6" s="32"/>
+      <c r="CL6" s="32"/>
+      <c r="CM6" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2325,39 +2321,39 @@
         <v>103</v>
       </c>
       <c r="BV7" s="24"/>
-      <c r="BW7" s="30" t="s">
+      <c r="BW7" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX7" s="31" t="s">
+      <c r="BX7" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY7" s="30" t="s">
+      <c r="BY7" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ7" s="30" t="s">
+      <c r="BZ7" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA7" s="30" t="s">
+      <c r="CA7" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB7" s="32"/>
+      <c r="CB7" s="31"/>
       <c r="CC7" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD7" s="32"/>
-      <c r="CE7" s="32"/>
-      <c r="CF7" s="32" t="s">
+      <c r="CD7" s="31"/>
+      <c r="CE7" s="31"/>
+      <c r="CF7" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG7" s="32"/>
-      <c r="CH7" s="32" t="s">
+      <c r="CG7" s="31"/>
+      <c r="CH7" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI7" s="32"/>
-      <c r="CJ7" s="33"/>
-      <c r="CK7" s="33"/>
-      <c r="CL7" s="33"/>
-      <c r="CM7" s="34" t="n">
+      <c r="CI7" s="31"/>
+      <c r="CJ7" s="32"/>
+      <c r="CK7" s="32"/>
+      <c r="CL7" s="32"/>
+      <c r="CM7" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2489,39 +2485,39 @@
         <v>103</v>
       </c>
       <c r="BV8" s="24"/>
-      <c r="BW8" s="30" t="s">
+      <c r="BW8" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX8" s="31" t="s">
+      <c r="BX8" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY8" s="30" t="s">
+      <c r="BY8" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ8" s="30" t="s">
+      <c r="BZ8" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA8" s="30" t="s">
+      <c r="CA8" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB8" s="32"/>
+      <c r="CB8" s="31"/>
       <c r="CC8" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD8" s="32"/>
-      <c r="CE8" s="32"/>
-      <c r="CF8" s="32" t="s">
+      <c r="CD8" s="31"/>
+      <c r="CE8" s="31"/>
+      <c r="CF8" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG8" s="32"/>
-      <c r="CH8" s="32" t="s">
+      <c r="CG8" s="31"/>
+      <c r="CH8" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI8" s="32"/>
-      <c r="CJ8" s="33"/>
-      <c r="CK8" s="33"/>
-      <c r="CL8" s="33"/>
-      <c r="CM8" s="34" t="n">
+      <c r="CI8" s="31"/>
+      <c r="CJ8" s="32"/>
+      <c r="CK8" s="32"/>
+      <c r="CL8" s="32"/>
+      <c r="CM8" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2653,39 +2649,39 @@
         <v>103</v>
       </c>
       <c r="BV9" s="24"/>
-      <c r="BW9" s="30" t="s">
+      <c r="BW9" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX9" s="31" t="s">
+      <c r="BX9" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY9" s="30" t="s">
+      <c r="BY9" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ9" s="30" t="s">
+      <c r="BZ9" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA9" s="30" t="s">
+      <c r="CA9" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB9" s="32"/>
+      <c r="CB9" s="31"/>
       <c r="CC9" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD9" s="32"/>
-      <c r="CE9" s="32"/>
-      <c r="CF9" s="32" t="s">
+      <c r="CD9" s="31"/>
+      <c r="CE9" s="31"/>
+      <c r="CF9" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG9" s="32"/>
-      <c r="CH9" s="32" t="s">
+      <c r="CG9" s="31"/>
+      <c r="CH9" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI9" s="32"/>
-      <c r="CJ9" s="33"/>
-      <c r="CK9" s="33"/>
-      <c r="CL9" s="33"/>
-      <c r="CM9" s="34" t="n">
+      <c r="CI9" s="31"/>
+      <c r="CJ9" s="32"/>
+      <c r="CK9" s="32"/>
+      <c r="CL9" s="32"/>
+      <c r="CM9" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2817,39 +2813,39 @@
         <v>103</v>
       </c>
       <c r="BV10" s="24"/>
-      <c r="BW10" s="30" t="s">
+      <c r="BW10" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX10" s="31" t="s">
+      <c r="BX10" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY10" s="30" t="s">
+      <c r="BY10" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ10" s="30" t="s">
+      <c r="BZ10" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA10" s="30" t="s">
+      <c r="CA10" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB10" s="32"/>
+      <c r="CB10" s="31"/>
       <c r="CC10" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD10" s="32"/>
-      <c r="CE10" s="32"/>
-      <c r="CF10" s="32" t="s">
+      <c r="CD10" s="31"/>
+      <c r="CE10" s="31"/>
+      <c r="CF10" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG10" s="32"/>
-      <c r="CH10" s="32" t="s">
+      <c r="CG10" s="31"/>
+      <c r="CH10" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI10" s="32"/>
-      <c r="CJ10" s="33"/>
-      <c r="CK10" s="33"/>
-      <c r="CL10" s="33"/>
-      <c r="CM10" s="34" t="n">
+      <c r="CI10" s="31"/>
+      <c r="CJ10" s="32"/>
+      <c r="CK10" s="32"/>
+      <c r="CL10" s="32"/>
+      <c r="CM10" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2981,39 +2977,39 @@
         <v>103</v>
       </c>
       <c r="BV11" s="24"/>
-      <c r="BW11" s="30" t="s">
+      <c r="BW11" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX11" s="31" t="s">
+      <c r="BX11" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY11" s="30" t="s">
+      <c r="BY11" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ11" s="30" t="s">
+      <c r="BZ11" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA11" s="30" t="s">
+      <c r="CA11" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB11" s="32"/>
+      <c r="CB11" s="31"/>
       <c r="CC11" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD11" s="32"/>
-      <c r="CE11" s="32"/>
-      <c r="CF11" s="32" t="s">
+      <c r="CD11" s="31"/>
+      <c r="CE11" s="31"/>
+      <c r="CF11" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG11" s="32"/>
-      <c r="CH11" s="32" t="s">
+      <c r="CG11" s="31"/>
+      <c r="CH11" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI11" s="32"/>
-      <c r="CJ11" s="33"/>
-      <c r="CK11" s="33"/>
-      <c r="CL11" s="33"/>
-      <c r="CM11" s="34" t="n">
+      <c r="CI11" s="31"/>
+      <c r="CJ11" s="32"/>
+      <c r="CK11" s="32"/>
+      <c r="CL11" s="32"/>
+      <c r="CM11" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3145,39 +3141,39 @@
         <v>103</v>
       </c>
       <c r="BV12" s="24"/>
-      <c r="BW12" s="30" t="s">
+      <c r="BW12" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX12" s="31" t="s">
+      <c r="BX12" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY12" s="30" t="s">
+      <c r="BY12" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ12" s="30" t="s">
+      <c r="BZ12" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA12" s="30" t="s">
+      <c r="CA12" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB12" s="32"/>
+      <c r="CB12" s="31"/>
       <c r="CC12" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD12" s="32"/>
-      <c r="CE12" s="32"/>
-      <c r="CF12" s="32" t="s">
+      <c r="CD12" s="31"/>
+      <c r="CE12" s="31"/>
+      <c r="CF12" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG12" s="32"/>
-      <c r="CH12" s="32" t="s">
+      <c r="CG12" s="31"/>
+      <c r="CH12" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI12" s="32"/>
-      <c r="CJ12" s="33"/>
-      <c r="CK12" s="33"/>
-      <c r="CL12" s="33"/>
-      <c r="CM12" s="34" t="n">
+      <c r="CI12" s="31"/>
+      <c r="CJ12" s="32"/>
+      <c r="CK12" s="32"/>
+      <c r="CL12" s="32"/>
+      <c r="CM12" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3309,39 +3305,39 @@
         <v>103</v>
       </c>
       <c r="BV13" s="24"/>
-      <c r="BW13" s="30" t="s">
+      <c r="BW13" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX13" s="31" t="s">
+      <c r="BX13" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY13" s="30" t="s">
+      <c r="BY13" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ13" s="30" t="s">
+      <c r="BZ13" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA13" s="30" t="s">
+      <c r="CA13" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB13" s="32"/>
+      <c r="CB13" s="31"/>
       <c r="CC13" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD13" s="32"/>
-      <c r="CE13" s="32"/>
-      <c r="CF13" s="32" t="s">
+      <c r="CD13" s="31"/>
+      <c r="CE13" s="31"/>
+      <c r="CF13" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG13" s="32"/>
-      <c r="CH13" s="32" t="s">
+      <c r="CG13" s="31"/>
+      <c r="CH13" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI13" s="32"/>
-      <c r="CJ13" s="33"/>
-      <c r="CK13" s="33"/>
-      <c r="CL13" s="33"/>
-      <c r="CM13" s="34" t="n">
+      <c r="CI13" s="31"/>
+      <c r="CJ13" s="32"/>
+      <c r="CK13" s="32"/>
+      <c r="CL13" s="32"/>
+      <c r="CM13" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3473,39 +3469,39 @@
         <v>103</v>
       </c>
       <c r="BV14" s="24"/>
-      <c r="BW14" s="30" t="s">
+      <c r="BW14" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX14" s="31" t="s">
+      <c r="BX14" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY14" s="30" t="s">
+      <c r="BY14" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ14" s="30" t="s">
+      <c r="BZ14" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA14" s="30" t="s">
+      <c r="CA14" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB14" s="32"/>
+      <c r="CB14" s="31"/>
       <c r="CC14" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD14" s="32"/>
-      <c r="CE14" s="32"/>
-      <c r="CF14" s="32" t="s">
+      <c r="CD14" s="31"/>
+      <c r="CE14" s="31"/>
+      <c r="CF14" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG14" s="32"/>
-      <c r="CH14" s="32" t="s">
+      <c r="CG14" s="31"/>
+      <c r="CH14" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI14" s="32"/>
-      <c r="CJ14" s="33"/>
-      <c r="CK14" s="33"/>
-      <c r="CL14" s="33"/>
-      <c r="CM14" s="34" t="n">
+      <c r="CI14" s="31"/>
+      <c r="CJ14" s="32"/>
+      <c r="CK14" s="32"/>
+      <c r="CL14" s="32"/>
+      <c r="CM14" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3637,39 +3633,39 @@
         <v>103</v>
       </c>
       <c r="BV15" s="24"/>
-      <c r="BW15" s="30" t="s">
+      <c r="BW15" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX15" s="31" t="s">
+      <c r="BX15" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY15" s="30" t="s">
+      <c r="BY15" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ15" s="30" t="s">
+      <c r="BZ15" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA15" s="30" t="s">
+      <c r="CA15" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB15" s="32"/>
+      <c r="CB15" s="31"/>
       <c r="CC15" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD15" s="32"/>
-      <c r="CE15" s="32"/>
-      <c r="CF15" s="32" t="s">
+      <c r="CD15" s="31"/>
+      <c r="CE15" s="31"/>
+      <c r="CF15" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG15" s="32"/>
-      <c r="CH15" s="32" t="s">
+      <c r="CG15" s="31"/>
+      <c r="CH15" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI15" s="32"/>
-      <c r="CJ15" s="33"/>
-      <c r="CK15" s="33"/>
-      <c r="CL15" s="33"/>
-      <c r="CM15" s="34" t="n">
+      <c r="CI15" s="31"/>
+      <c r="CJ15" s="32"/>
+      <c r="CK15" s="32"/>
+      <c r="CL15" s="32"/>
+      <c r="CM15" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3801,39 +3797,39 @@
         <v>103</v>
       </c>
       <c r="BV16" s="24"/>
-      <c r="BW16" s="30" t="s">
+      <c r="BW16" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX16" s="31" t="s">
+      <c r="BX16" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY16" s="30" t="s">
+      <c r="BY16" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ16" s="30" t="s">
+      <c r="BZ16" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA16" s="30" t="s">
+      <c r="CA16" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB16" s="32"/>
+      <c r="CB16" s="31"/>
       <c r="CC16" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD16" s="32"/>
-      <c r="CE16" s="32"/>
-      <c r="CF16" s="32" t="s">
+      <c r="CD16" s="31"/>
+      <c r="CE16" s="31"/>
+      <c r="CF16" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG16" s="32"/>
-      <c r="CH16" s="32" t="s">
+      <c r="CG16" s="31"/>
+      <c r="CH16" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI16" s="32"/>
-      <c r="CJ16" s="33"/>
-      <c r="CK16" s="33"/>
-      <c r="CL16" s="33"/>
-      <c r="CM16" s="34" t="n">
+      <c r="CI16" s="31"/>
+      <c r="CJ16" s="32"/>
+      <c r="CK16" s="32"/>
+      <c r="CL16" s="32"/>
+      <c r="CM16" s="33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3965,39 +3961,39 @@
         <v>103</v>
       </c>
       <c r="BV17" s="24"/>
-      <c r="BW17" s="30" t="s">
+      <c r="BW17" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="BX17" s="31" t="s">
+      <c r="BX17" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="BY17" s="30" t="s">
+      <c r="BY17" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="BZ17" s="30" t="s">
+      <c r="BZ17" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="CA17" s="30" t="s">
+      <c r="CA17" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="CB17" s="32"/>
+      <c r="CB17" s="31"/>
       <c r="CC17" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="CD17" s="32"/>
-      <c r="CE17" s="32"/>
-      <c r="CF17" s="32" t="s">
+      <c r="CD17" s="31"/>
+      <c r="CE17" s="31"/>
+      <c r="CF17" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="CG17" s="32"/>
-      <c r="CH17" s="32" t="s">
+      <c r="CG17" s="31"/>
+      <c r="CH17" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="CI17" s="32"/>
-      <c r="CJ17" s="33"/>
-      <c r="CK17" s="33"/>
-      <c r="CL17" s="33"/>
-      <c r="CM17" s="34" t="n">
+      <c r="CI17" s="31"/>
+      <c r="CJ17" s="32"/>
+      <c r="CK17" s="32"/>
+      <c r="CL17" s="32"/>
+      <c r="CM17" s="33" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>